<commit_message>
Add database connection for component.equipment_penetration_rates
</commit_message>
<xml_diff>
--- a/test_data/installation/equipment_perf_rates.xlsx
+++ b/test_data/installation/equipment_perf_rates.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-core\test_data\installation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="penet" sheetId="1" r:id="rId1"/>
@@ -99,25 +104,25 @@
     <t>Cost Contingency [%]</t>
   </si>
   <si>
-    <t>Drilling rig [m/h]</t>
-  </si>
-  <si>
-    <t>Hammer [m/h]</t>
-  </si>
-  <si>
-    <t>Vibro driver [m/h]</t>
-  </si>
-  <si>
-    <t>ROV with suction pump [m/h]</t>
-  </si>
-  <si>
-    <t>ROV with jetting [m/h]</t>
+    <t>Drilling rig</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Vibro driver</t>
+  </si>
+  <si>
+    <t>ROV with suction pump</t>
+  </si>
+  <si>
+    <t>ROV with jetting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,6 +202,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -491,7 +499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,27 +510,27 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -563,7 +571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -604,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -645,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -686,7 +694,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -727,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -781,24 +789,24 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -839,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -880,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -921,7 +929,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -962,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1016,19 +1024,19 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1044,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1052,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1052,7 +1060,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1068,7 +1076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>

</xml_diff>